<commit_message>
Mulitple updates to stanpumpR
</commit_message>
<xml_diff>
--- a/data/Drug Defaults.xlsx
+++ b/data/Drug Defaults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\StanpumpR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\StanpumpR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD71CD7-9345-428A-BEC8-90C5507E2D3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9029292C-719E-49A4-A43C-5F4195CA8C33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" xr2:uid="{F1EDE105-E79D-43EB-8BB3-A0EECCFD5A7A}"/>
+    <workbookView xWindow="-12188" yWindow="-15188" windowWidth="12151" windowHeight="21323" xr2:uid="{F1EDE105-E79D-43EB-8BB3-A0EECCFD5A7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="63">
   <si>
     <t>propofol</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>mg,mg/kg,mg/hr,mg/kg/hr,mg PO,mg IM,mg IN</t>
+  </si>
+  <si>
+    <t>mcg,mcg/kg,mg,mg/kg,mcg/min,mcg/kg/min,mg/min,mg/kg/min</t>
   </si>
 </sst>
 </file>
@@ -582,7 +585,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1223,7 +1226,7 @@
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="G17" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Update on January 28, 2020
</commit_message>
<xml_diff>
--- a/data/Drug Defaults.xlsx
+++ b/data/Drug Defaults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\StanpumpR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FF40BB-808D-4457-AC57-BD665A967EF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202D951A-E261-44FC-8F6E-017FE888806C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" xr2:uid="{F1EDE105-E79D-43EB-8BB3-A0EECCFD5A7A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{F1EDE105-E79D-43EB-8BB3-A0EECCFD5A7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>mg,mg/kg/hr</t>
   </si>
   <si>
-    <t>mcg,mcg/min</t>
-  </si>
-  <si>
     <t>Default Units</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>mg,mg/kg,mg/hr,mg/kg/hr</t>
+  </si>
+  <si>
+    <t>mcg,mg,mg/kg,mcg/min</t>
   </si>
 </sst>
 </file>
@@ -609,7 +609,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -639,7 +639,7 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
         <v>43</v>
@@ -648,22 +648,22 @@
         <v>28</v>
       </c>
       <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
         <v>53</v>
       </c>
-      <c r="I1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" t="s">
-        <v>54</v>
-      </c>
       <c r="K1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
@@ -683,7 +683,7 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -704,7 +704,7 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
@@ -724,7 +724,7 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
         <v>38</v>
@@ -745,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
         <v>33</v>
@@ -786,7 +786,7 @@
         <v>0.6</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
@@ -806,7 +806,7 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
         <v>33</v>
@@ -827,7 +827,7 @@
         <v>39</v>
       </c>
       <c r="M5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
@@ -847,7 +847,7 @@
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
         <v>33</v>
@@ -868,7 +868,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="M6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
@@ -909,7 +909,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="M7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
@@ -950,7 +950,7 @@
         <v>0.25</v>
       </c>
       <c r="M8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
@@ -970,7 +970,7 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" t="s">
         <v>32</v>
@@ -991,7 +991,7 @@
         <v>1.5</v>
       </c>
       <c r="M9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
@@ -1032,7 +1032,7 @@
         <v>0.06</v>
       </c>
       <c r="M10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
@@ -1052,7 +1052,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G11" t="s">
         <v>29</v>
@@ -1073,7 +1073,7 @@
         <v>0.1</v>
       </c>
       <c r="M11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
@@ -1093,7 +1093,7 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
         <v>37</v>
@@ -1114,7 +1114,7 @@
         <v>0.4</v>
       </c>
       <c r="M12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
@@ -1134,7 +1134,7 @@
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
         <v>36</v>
@@ -1155,7 +1155,7 @@
         <v>0.04</v>
       </c>
       <c r="M13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
@@ -1196,7 +1196,7 @@
         <v>0.4</v>
       </c>
       <c r="M14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
@@ -1237,7 +1237,7 @@
         <v>0.5</v>
       </c>
       <c r="M15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
@@ -1278,7 +1278,7 @@
         <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.45">
@@ -1298,7 +1298,7 @@
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G17" t="s">
         <v>35</v>
@@ -1319,7 +1319,7 @@
         <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.45">
@@ -1339,7 +1339,7 @@
         <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
         <v>42</v>
@@ -1360,7 +1360,7 @@
         <v>0.05</v>
       </c>
       <c r="M18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.45">
@@ -1371,10 +1371,10 @@
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G19" t="s">
         <v>32</v>
@@ -1395,7 +1395,7 @@
         <v>10</v>
       </c>
       <c r="M19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>